<commit_message>
Update to adapt to each big 4 banks
</commit_message>
<xml_diff>
--- a/Westpac_TD.xlsx
+++ b/Westpac_TD.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">           Term Interest paid at maturity Interest paid monthly
 0  1 &lt; 2 months                     0.15%                 0.15%
@@ -22,6 +22,28 @@
 2  3 &lt; 4 months                     0.70%                 0.70%
 3  4 &lt; 5 months                     0.65%                 0.65%
 4  5 &lt; 6 months                     0.65%                 0.65%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             Term Interest paid at maturity Interest paid monthly
+0    6 &lt; 7 months                     0.65%                 0.65%
+1    7 &lt; 8 months                     0.70%                 0.70%
+2    8 &lt; 9 months                     0.70%                 0.70%
+3   9 &lt; 10 months                     0.65%                 0.65%
+4  10 &lt; 11 months                     0.70%                 0.70%
+5  11 &lt; 12 months                     0.65%                 0.65%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             Term Interest paid yearly Interest paid monthly
+0  12 &lt; 24 months                0.85%                 0.85%
+1  24 &lt; 36 months                1.00%                 1.00%
+2  36 &lt; 48 months                1.00%                 1.00%
+3  48 &lt; 60 months                1.00%                 1.00%
+4       60 months                1.00%                 1.00%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  $5,000 &lt; $10,000  ... $100,000 &lt; $25,000,000
+0            0.05%  ...                  0.05%
+[1 rows x 5 columns]</t>
   </si>
 </sst>
 </file>
@@ -379,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -395,6 +417,21 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>